<commit_message>
Updates and additional data
</commit_message>
<xml_diff>
--- a/macro_tz.xlsx
+++ b/macro_tz.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/f6a97429bfd31d15/Documents/GitHub/Stock_Markets/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\marvi\OneDrive\Documents\GitHub\Stock_Markets\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="3" documentId="13_ncr:1_{8945F7FE-088A-4A80-9AF4-8F786EC111F0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{D210A255-9EA3-49B0-80E7-DE239000A150}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C259B0AF-B692-4433-96F6-832A31814215}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11040" xr2:uid="{3E751FD4-9AFA-4107-8DDE-1E44AA23F6CE}"/>
   </bookViews>
@@ -415,7 +415,7 @@
   <dimension ref="A1:F295"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H14" sqref="H14"/>
+      <selection activeCell="N16" sqref="N16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -426,6 +426,7 @@
     <col min="4" max="4" width="12.7109375" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="16.85546875" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="8.140625" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="11" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:6" x14ac:dyDescent="0.25">
@@ -456,7 +457,7 @@
         <v>0.24</v>
       </c>
       <c r="C2">
-        <v>0.28604118993135202</v>
+        <v>72.488147403574402</v>
       </c>
       <c r="D2">
         <v>1.5491720432712499</v>
@@ -476,7 +477,7 @@
         <v>0.12</v>
       </c>
       <c r="C3">
-        <v>0.22818026240728501</v>
+        <v>72.488147403574402</v>
       </c>
       <c r="D3">
         <v>1.7404106130861501</v>
@@ -496,7 +497,7 @@
         <v>0.3</v>
       </c>
       <c r="C4">
-        <v>0.284575981787139</v>
+        <v>72.529427669749595</v>
       </c>
       <c r="D4">
         <v>1.8426207998953701</v>
@@ -516,7 +517,7 @@
         <v>0.73</v>
       </c>
       <c r="C5">
-        <v>0.34052213393872699</v>
+        <v>72.777109266800593</v>
       </c>
       <c r="D5">
         <v>2.67599038238358</v>
@@ -536,7 +537,7 @@
         <v>0</v>
       </c>
       <c r="C6">
-        <v>-0.11312217194570801</v>
+        <v>72.859669799150893</v>
       </c>
       <c r="D6">
         <v>1.7151774759723399</v>
@@ -556,7 +557,7 @@
         <v>0</v>
       </c>
       <c r="C7">
-        <v>0</v>
+        <v>72.900950065326001</v>
       </c>
       <c r="D7">
         <v>1.1828446049785699</v>
@@ -576,7 +577,7 @@
         <v>0.3</v>
       </c>
       <c r="C8">
-        <v>0.16987542468855699</v>
+        <v>73.107351396201807</v>
       </c>
       <c r="D8">
         <v>2.39370686970687</v>
@@ -596,7 +597,7 @@
         <v>0.24</v>
       </c>
       <c r="C9">
-        <v>0.113058224985859</v>
+        <v>73.189911928552107</v>
       </c>
       <c r="D9">
         <v>2.3615824284601001</v>
@@ -616,7 +617,7 @@
         <v>0.48</v>
       </c>
       <c r="C10">
-        <v>0.33879164313947402</v>
+        <v>73.396313259427899</v>
       </c>
       <c r="D10">
         <v>2.4805631178883298</v>
@@ -636,7 +637,7 @@
         <v>0.18</v>
       </c>
       <c r="C11">
-        <v>0.33764772087788902</v>
+        <v>73.520154057953405</v>
       </c>
       <c r="D11">
         <v>1.6936058652114001</v>
@@ -656,7 +657,7 @@
         <v>0.06</v>
       </c>
       <c r="C12">
-        <v>5.6085249579363998E-2</v>
+        <v>73.643994856478798</v>
       </c>
       <c r="D12">
         <v>2.1877552724092602</v>
@@ -676,7 +677,7 @@
         <v>0</v>
       </c>
       <c r="C13">
-        <v>-0.112107623318392</v>
+        <v>73.767835655004305</v>
       </c>
       <c r="D13">
         <v>2.60237344537454</v>
@@ -696,7 +697,7 @@
         <v>0.3</v>
       </c>
       <c r="C14">
-        <v>0.336700336700342</v>
+        <v>74.015517252055204</v>
       </c>
       <c r="D14">
         <v>3.8517711261752301</v>
@@ -716,7 +717,7 @@
         <v>0.59</v>
       </c>
       <c r="C15">
-        <v>0.39149888143176098</v>
+        <v>74.056797518230397</v>
       </c>
       <c r="D15">
         <v>2.7855839250199299</v>
@@ -736,7 +737,7 @@
         <v>0.82</v>
       </c>
       <c r="C16">
-        <v>0.55710306406684096</v>
+        <v>74.304479115281396</v>
       </c>
       <c r="D16">
         <v>3.4168087758401602</v>
@@ -756,7 +757,7 @@
         <v>0.06</v>
       </c>
       <c r="C17">
-        <v>0.22160664819945899</v>
+        <v>74.428319913806803</v>
       </c>
       <c r="D17">
         <v>2.2769012664177701</v>
@@ -776,7 +777,7 @@
         <v>0.12</v>
       </c>
       <c r="C18">
-        <v>0</v>
+        <v>74.593440978507402</v>
       </c>
       <c r="D18">
         <v>2.8535338447598599</v>
@@ -796,7 +797,7 @@
         <v>0.52</v>
       </c>
       <c r="C19">
-        <v>5.5279159756774998E-2</v>
+        <v>74.758562043208101</v>
       </c>
       <c r="D19">
         <v>3.1425345027014102</v>
@@ -816,7 +817,7 @@
         <v>0.23</v>
       </c>
       <c r="C20">
-        <v>0.16574585635360101</v>
+        <v>74.923683107908701</v>
       </c>
       <c r="D20">
         <v>3.4363633527404698</v>
@@ -836,7 +837,7 @@
         <v>0</v>
       </c>
       <c r="C21">
-        <v>0.22062879205734701</v>
+        <v>75.088804172609301</v>
       </c>
       <c r="D21">
         <v>2.8757006150934301</v>
@@ -856,7 +857,7 @@
         <v>0.52</v>
       </c>
       <c r="C22">
-        <v>0.33021463951569002</v>
+        <v>75.2539252373099</v>
       </c>
       <c r="D22">
         <v>3.0687342335299999</v>
@@ -876,7 +877,7 @@
         <v>0.17</v>
       </c>
       <c r="C23">
-        <v>0.27427317608338098</v>
+        <v>75.377766035835407</v>
       </c>
       <c r="D23">
         <v>2.7010732653574498</v>
@@ -896,7 +897,7 @@
         <v>0.06</v>
       </c>
       <c r="C24">
-        <v>0.109409190371983</v>
+        <v>75.584167366711199</v>
       </c>
       <c r="D24">
         <v>2.6517739997200098</v>
@@ -916,7 +917,7 @@
         <v>-0.06</v>
       </c>
       <c r="C25">
-        <v>-0.10928961748633099</v>
+        <v>75.666727899061499</v>
       </c>
       <c r="D25">
         <v>3.2964610225159099</v>
@@ -936,7 +937,7 @@
         <v>0.63</v>
       </c>
       <c r="C26">
-        <v>0.38293216630196297</v>
+        <v>75.914409496112398</v>
       </c>
       <c r="D26">
         <v>4.0764778317574004</v>
@@ -956,7 +957,7 @@
         <v>0.4</v>
       </c>
       <c r="C27">
-        <v>0.490463215258856</v>
+        <v>76.120810826988205</v>
       </c>
       <c r="D27">
         <v>2.8367889543748901</v>
@@ -976,7 +977,7 @@
         <v>0.23</v>
       </c>
       <c r="C28">
-        <v>0.48806941431671802</v>
+        <v>76.244651625513697</v>
       </c>
       <c r="D28">
         <v>2.9921466051607801</v>
@@ -996,7 +997,7 @@
         <v>0.4</v>
       </c>
       <c r="C29">
-        <v>0.16189962223419599</v>
+        <v>76.409772690214297</v>
       </c>
       <c r="D29">
         <v>3.1446330881268199</v>
@@ -1016,7 +1017,7 @@
         <v>0.45</v>
       </c>
       <c r="C30">
-        <v>-5.3879310344830803E-2</v>
+        <v>76.492333222564596</v>
       </c>
       <c r="D30">
         <v>3.50111619196587</v>
@@ -1036,7 +1037,7 @@
         <v>0.17</v>
       </c>
       <c r="C31">
-        <v>0.21563342318060599</v>
+        <v>76.781295085790703</v>
       </c>
       <c r="D31">
         <v>3.5218003147550201</v>
@@ -1056,7 +1057,7 @@
         <v>-0.28000000000000003</v>
       </c>
       <c r="C32">
-        <v>0.16137708445400301</v>
+        <v>76.946416150491402</v>
       </c>
       <c r="D32">
         <v>2.4350411076885399</v>
@@ -1076,7 +1077,7 @@
         <v>0</v>
       </c>
       <c r="C33">
-        <v>0.21482277121374699</v>
+        <v>77.070256949016795</v>
       </c>
       <c r="D33">
         <v>3.80544284558475</v>
@@ -1096,7 +1097,7 @@
         <v>0.45</v>
       </c>
       <c r="C34">
-        <v>0.26795284030010902</v>
+        <v>77.235378013717394</v>
       </c>
       <c r="D34">
         <v>2.78250757475318</v>
@@ -1116,7 +1117,7 @@
         <v>-0.34</v>
       </c>
       <c r="C35">
-        <v>0.267236771779784</v>
+        <v>77.359218812242901</v>
       </c>
       <c r="D35">
         <v>4.1840765820082098</v>
@@ -1136,7 +1137,7 @@
         <v>-0.17</v>
       </c>
       <c r="C36">
-        <v>0.26652452025588003</v>
+        <v>77.648180675469007</v>
       </c>
       <c r="D36">
         <v>3.4431714115967198</v>
@@ -1156,7 +1157,7 @@
         <v>-0.39</v>
       </c>
       <c r="C37">
-        <v>-0.15948963317383899</v>
+        <v>77.772021473994499</v>
       </c>
       <c r="D37">
         <v>2.4752860319994201</v>
@@ -1176,7 +1177,7 @@
         <v>0.23</v>
       </c>
       <c r="C38">
-        <v>0.2129925452609</v>
+        <v>77.895862272519906</v>
       </c>
       <c r="D38">
         <v>2.7615896715014898</v>
@@ -1196,7 +1197,7 @@
         <v>0.4</v>
       </c>
       <c r="C39">
-        <v>0.53134962805526398</v>
+        <v>78.060983337220605</v>
       </c>
       <c r="D39">
         <v>3.38352407504046</v>
@@ -1216,7 +1217,7 @@
         <v>0.56000000000000005</v>
       </c>
       <c r="C40">
-        <v>0.31712473572939198</v>
+        <v>78.102263603395699</v>
       </c>
       <c r="D40">
         <v>2.8726214230370899</v>
@@ -1236,7 +1237,7 @@
         <v>0.56000000000000005</v>
       </c>
       <c r="C41">
-        <v>0.26343519494206002</v>
+        <v>78.308664934271505</v>
       </c>
       <c r="D41">
         <v>2.67648214481753</v>
@@ -1256,7 +1257,7 @@
         <v>0</v>
       </c>
       <c r="C42">
-        <v>-5.2548607461919597E-2</v>
+        <v>78.432505732796997</v>
       </c>
       <c r="D42">
         <v>2.4201984381925699</v>
@@ -1276,7 +1277,7 @@
         <v>0.06</v>
       </c>
       <c r="C43">
-        <v>-5.2576235541538403E-2</v>
+        <v>78.515066265147297</v>
       </c>
       <c r="D43">
         <v>2.5025331988713</v>
@@ -1296,7 +1297,7 @@
         <v>0.11</v>
       </c>
       <c r="C44">
-        <v>0.10520778537613799</v>
+        <v>78.638907063672804</v>
       </c>
       <c r="D44">
         <v>2.2450552311313401</v>
@@ -1316,7 +1317,7 @@
         <v>0.33</v>
       </c>
       <c r="C45">
-        <v>0.36784025223331002</v>
+        <v>78.886588660723703</v>
       </c>
       <c r="D45">
         <v>2.28572177593909</v>
@@ -1336,7 +1337,7 @@
         <v>0.17</v>
       </c>
       <c r="C46">
-        <v>0.15706806282722</v>
+        <v>78.969149193074003</v>
       </c>
       <c r="D46">
         <v>2.7177978977574799</v>
@@ -1356,7 +1357,7 @@
         <v>0.17</v>
       </c>
       <c r="C47">
-        <v>0.26136957658128801</v>
+        <v>79.051709725424303</v>
       </c>
       <c r="D47">
         <v>2.3139030753389398</v>
@@ -1376,7 +1377,7 @@
         <v>0</v>
       </c>
       <c r="C48">
-        <v>0</v>
+        <v>79.216830790124902</v>
       </c>
       <c r="D48">
         <v>1.91097600745183</v>
@@ -1396,7 +1397,7 @@
         <v>-0.22</v>
       </c>
       <c r="C49">
-        <v>-0.20855057351407599</v>
+        <v>79.299391322475302</v>
       </c>
       <c r="D49">
         <v>3.01261428455381</v>
@@ -1416,7 +1417,7 @@
         <v>0.44</v>
       </c>
       <c r="C50">
-        <v>0.20898641588296599</v>
+        <v>79.423232121000694</v>
       </c>
       <c r="D50">
         <v>2.1813904276981599</v>
@@ -1436,7 +1437,7 @@
         <v>0.77</v>
       </c>
       <c r="C51">
-        <v>0.36496350364962898</v>
+        <v>79.464512387175901</v>
       </c>
       <c r="D51">
         <v>1.9758302344968099</v>
@@ -1456,7 +1457,7 @@
         <v>0.6</v>
       </c>
       <c r="C52">
-        <v>0.259740259740247</v>
+        <v>79.464512387175901</v>
       </c>
       <c r="D52">
         <v>1.1262118092594899</v>
@@ -1476,7 +1477,7 @@
         <v>-0.22</v>
       </c>
       <c r="C53">
-        <v>5.1813471502607698E-2</v>
+        <v>79.464512387175901</v>
       </c>
       <c r="D53">
         <v>0.55303689047201399</v>
@@ -1496,7 +1497,7 @@
         <v>-0.16</v>
       </c>
       <c r="C54">
-        <v>5.1786639047115002E-2</v>
+        <v>79.629633451876501</v>
       </c>
       <c r="D54">
         <v>1.0757881864280301</v>
@@ -1516,7 +1517,7 @@
         <v>0.11</v>
       </c>
       <c r="C55">
-        <v>-0.103519668737066</v>
+        <v>79.670913718051594</v>
       </c>
       <c r="D55">
         <v>1.12305963544221</v>
@@ -1536,7 +1537,7 @@
         <v>0.11</v>
       </c>
       <c r="C56">
-        <v>0.103626943005188</v>
+        <v>79.836034782752293</v>
       </c>
       <c r="D56">
         <v>2.6710731226570998</v>
@@ -1556,7 +1557,7 @@
         <v>0.38</v>
       </c>
       <c r="C57">
-        <v>0.15527950310559899</v>
+        <v>79.918595315102607</v>
       </c>
       <c r="D57">
         <v>2.3574142692481801</v>
@@ -1576,7 +1577,7 @@
         <v>0.33</v>
       </c>
       <c r="C58">
-        <v>5.1679586563296701E-2</v>
+        <v>79.959875581277799</v>
       </c>
       <c r="D58">
         <v>2.02226514469577</v>
@@ -1596,7 +1597,7 @@
         <v>-0.11</v>
       </c>
       <c r="C59">
-        <v>0.36157024793389198</v>
+        <v>80.083716379803207</v>
       </c>
       <c r="D59">
         <v>2.0958674943976101</v>
@@ -1616,7 +1617,7 @@
         <v>-0.27</v>
       </c>
       <c r="C60">
-        <v>-0.20586721564590699</v>
+        <v>80.083716379803207</v>
       </c>
       <c r="D60">
         <v>1.18636241164811</v>
@@ -1636,7 +1637,7 @@
         <v>-0.11</v>
       </c>
       <c r="C61">
-        <v>-0.15471892728211301</v>
+        <v>80.166276912153506</v>
       </c>
       <c r="D61">
         <v>1.79882233944806</v>
@@ -1656,7 +1657,7 @@
         <v>0.49</v>
       </c>
       <c r="C62">
-        <v>0.206611570247932</v>
+        <v>80.331397976854205</v>
       </c>
       <c r="D62">
         <v>2.2200747059839498</v>
@@ -1676,7 +1677,7 @@
         <v>0.54</v>
       </c>
       <c r="C63">
-        <v>0.46391752577320999</v>
+        <v>80.455238775379598</v>
       </c>
       <c r="D63">
         <v>2.9126545534697401</v>
@@ -1696,7 +1697,7 @@
         <v>0.64</v>
       </c>
       <c r="C64">
-        <v>0.61570035915853805</v>
+        <v>80.702920372430597</v>
       </c>
       <c r="D64">
         <v>2.7344022682197799</v>
@@ -1716,7 +1717,7 @@
         <v>0.32</v>
       </c>
       <c r="C65">
-        <v>0.20397756246812701</v>
+        <v>80.868041437131197</v>
       </c>
       <c r="D65">
         <v>2.5383819269539298</v>
@@ -1736,7 +1737,7 @@
         <v>0.59</v>
       </c>
       <c r="C66">
-        <v>0</v>
+        <v>80.991882235656604</v>
       </c>
       <c r="D66">
         <v>3.2174948905270599</v>
@@ -1756,7 +1757,7 @@
         <v>0.32</v>
       </c>
       <c r="C67">
-        <v>5.0890585241733302E-2</v>
+        <v>81.157003300357303</v>
       </c>
       <c r="D67">
         <v>2.7249314488472498</v>
@@ -1776,7 +1777,7 @@
         <v>-0.16</v>
       </c>
       <c r="C68">
-        <v>0</v>
+        <v>81.239563832707603</v>
       </c>
       <c r="D68">
         <v>1.7711369595551301</v>
@@ -1796,7 +1797,7 @@
         <v>0.05</v>
       </c>
       <c r="C69">
-        <v>0.10172939979654699</v>
+        <v>81.280844098882795</v>
       </c>
       <c r="D69">
         <v>2.8732374517403501</v>
@@ -1816,7 +1817,7 @@
         <v>0.21</v>
       </c>
       <c r="C70">
-        <v>0.30487804878049202</v>
+        <v>81.528525695933695</v>
       </c>
       <c r="D70">
         <v>2.1466349952753001</v>
@@ -1836,7 +1837,7 @@
         <v>0.53</v>
       </c>
       <c r="C71">
-        <v>0.40526849037485702</v>
+        <v>81.693646760634294</v>
       </c>
       <c r="D71">
         <v>2.6605010937276199</v>
@@ -1856,7 +1857,7 @@
         <v>0.05</v>
       </c>
       <c r="C72">
-        <v>-5.0454086781018703E-2</v>
+        <v>81.858767825334894</v>
       </c>
       <c r="D72">
         <v>1.4800663055379</v>
@@ -1876,7 +1877,7 @@
         <v>-0.37</v>
       </c>
       <c r="C73">
-        <v>-0.151438667339723</v>
+        <v>81.982608623860401</v>
       </c>
       <c r="D73">
         <v>1.9152497260885599</v>
@@ -1896,7 +1897,7 @@
         <v>0.21</v>
       </c>
       <c r="C74">
-        <v>0.30333670374114402</v>
+        <v>82.147729688561</v>
       </c>
       <c r="D74">
         <v>3.4217591363454098</v>
@@ -1916,7 +1917,7 @@
         <v>0.57999999999999996</v>
       </c>
       <c r="C75">
-        <v>0.55443548387097397</v>
+        <v>82.3128507532616</v>
       </c>
       <c r="D75">
         <v>3.3040022907410398</v>
@@ -1936,7 +1937,7 @@
         <v>0.78</v>
       </c>
       <c r="C76">
-        <v>0.60150375939849199</v>
+        <v>82.601812616487805</v>
       </c>
       <c r="D76">
         <v>1.89717939501216</v>
@@ -1956,7 +1957,7 @@
         <v>0.67</v>
       </c>
       <c r="C77">
-        <v>9.9651220727446504E-2</v>
+        <v>82.643092882662899</v>
       </c>
       <c r="D77">
         <v>2.0964790133565199</v>
@@ -1976,7 +1977,7 @@
         <v>-0.1</v>
       </c>
       <c r="C78">
-        <v>-4.9776007964164301E-2</v>
+        <v>82.766933681188405</v>
       </c>
       <c r="D78">
         <v>3.1684623516185599</v>
@@ -1996,7 +1997,7 @@
         <v>0.05</v>
       </c>
       <c r="C79">
-        <v>-9.9601593625503998E-2</v>
+        <v>82.808213947363498</v>
       </c>
       <c r="D79">
         <v>1.62477538920178</v>
@@ -2016,7 +2017,7 @@
         <v>0.46</v>
       </c>
       <c r="C80">
-        <v>9.9700897308081807E-2</v>
+        <v>82.932054745889005</v>
       </c>
       <c r="D80">
         <v>3.0286455734746398</v>
@@ -2036,7 +2037,7 @@
         <v>0.51</v>
       </c>
       <c r="C81">
-        <v>9.9601593625517404E-2</v>
+        <v>83.014615278239305</v>
       </c>
       <c r="D81">
         <v>2.22215620270876</v>
@@ -2056,7 +2057,7 @@
         <v>1.22</v>
       </c>
       <c r="C82">
-        <v>0.14925373134327899</v>
+        <v>83.097175810589604</v>
       </c>
       <c r="D82">
         <v>4.02470724061161</v>
@@ -2076,7 +2077,7 @@
         <v>0.2</v>
       </c>
       <c r="C83">
-        <v>0.496770988574257</v>
+        <v>83.386137673815696</v>
       </c>
       <c r="D83">
         <v>3.3315751559861799</v>
@@ -2096,7 +2097,7 @@
         <v>-0.8</v>
       </c>
       <c r="C84">
-        <v>0</v>
+        <v>83.592539004691503</v>
       </c>
       <c r="D84">
         <v>2.8369119481422498</v>
@@ -2116,7 +2117,7 @@
         <v>-0.4</v>
       </c>
       <c r="C85">
-        <v>-9.8863074641627302E-2</v>
+        <v>83.716379803216995</v>
       </c>
       <c r="D85">
         <v>2.2048931992040099</v>
@@ -2136,7 +2137,7 @@
         <v>0.76</v>
       </c>
       <c r="C86">
-        <v>0.24740227610092799</v>
+        <v>83.881500867917595</v>
       </c>
       <c r="D86">
         <v>2.8843218662388601</v>
@@ -2156,7 +2157,7 @@
         <v>0.2</v>
       </c>
       <c r="C87">
-        <v>0.493583415597252</v>
+        <v>84.046621932618194</v>
       </c>
       <c r="D87">
         <v>2.0720208737155601</v>
@@ -2176,7 +2177,7 @@
         <v>0.55000000000000004</v>
       </c>
       <c r="C88">
-        <v>0.63850687622789704</v>
+        <v>84.3355837958443</v>
       </c>
       <c r="D88">
         <v>3.0821825136096299</v>
@@ -2196,7 +2197,7 @@
         <v>0.85</v>
       </c>
       <c r="C89">
-        <v>0.29282576866764698</v>
+        <v>84.541985126720107</v>
       </c>
       <c r="D89">
         <v>2.8870316165126</v>
@@ -2216,7 +2217,7 @@
         <v>0.5</v>
       </c>
       <c r="C90">
-        <v>9.7323600973228799E-2</v>
+        <v>84.789666723771006</v>
       </c>
       <c r="D90">
         <v>4.2881606845839304</v>
@@ -2236,7 +2237,7 @@
         <v>0.2</v>
       </c>
       <c r="C91">
-        <v>9.7228974234327706E-2</v>
+        <v>84.996068054646798</v>
       </c>
       <c r="D91">
         <v>3.19983083499134</v>
@@ -2256,7 +2257,7 @@
         <v>0.3</v>
       </c>
       <c r="C92">
-        <v>0.14570179698882499</v>
+        <v>85.161189119347398</v>
       </c>
       <c r="D92">
         <v>3.0539305241528298</v>
@@ -2276,7 +2277,7 @@
         <v>0.2</v>
       </c>
       <c r="C93">
-        <v>0.24248302618815501</v>
+        <v>85.367590450223204</v>
       </c>
       <c r="D93">
         <v>4.6213703967792101</v>
@@ -2296,7 +2297,7 @@
         <v>-0.49</v>
       </c>
       <c r="C94">
-        <v>0.24189646831157699</v>
+        <v>85.532711514923804</v>
       </c>
       <c r="D94">
         <v>2.1062637733366598</v>
@@ -2316,7 +2317,7 @@
         <v>-0.54</v>
       </c>
       <c r="C95">
-        <v>0.28957528957530698</v>
+        <v>85.697832579624503</v>
       </c>
       <c r="D95">
         <v>3.6506970400157699</v>
@@ -2336,7 +2337,7 @@
         <v>-0.15</v>
       </c>
       <c r="C96">
-        <v>-9.6246390760365202E-2</v>
+        <v>85.780393111974803</v>
       </c>
       <c r="D96">
         <v>3.02469916751935</v>
@@ -2356,7 +2357,7 @@
         <v>0.15</v>
       </c>
       <c r="C97">
-        <v>-0.14450867052022701</v>
+        <v>85.904233910500196</v>
       </c>
       <c r="D97">
         <v>2.7255465438013302</v>
@@ -2376,7 +2377,7 @@
         <v>0.31</v>
       </c>
       <c r="C98">
-        <v>0.342016401350687</v>
+        <v>86.110635241376002</v>
       </c>
       <c r="D98">
         <v>2.9644102631689102</v>
@@ -2396,7 +2397,7 @@
         <v>0.54</v>
       </c>
       <c r="C99">
-        <v>0.53026551735743399</v>
+        <v>86.3314846654131</v>
       </c>
       <c r="D99">
         <v>4.4470256400193398</v>
@@ -2416,7 +2417,7 @@
         <v>0.91</v>
       </c>
       <c r="C100">
-        <v>0.38783044492902802</v>
+        <v>86.448307818688804</v>
       </c>
       <c r="D100">
         <v>2.6885311218425199</v>
@@ -2436,7 +2437,7 @@
         <v>0.65</v>
       </c>
       <c r="C101">
-        <v>0.18482967564297301</v>
+        <v>86.584119894405106</v>
       </c>
       <c r="D101">
         <v>2.3683253683680201</v>
@@ -2456,7 +2457,7 @@
         <v>0.61</v>
       </c>
       <c r="C102">
-        <v>2.3774315180827101E-3</v>
+        <v>86.712501522209806</v>
       </c>
       <c r="D102">
         <v>2.35349143799752</v>
@@ -2476,7 +2477,7 @@
         <v>0.19</v>
       </c>
       <c r="C103">
-        <v>7.51250499248831E-2</v>
+        <v>86.850377611234805</v>
       </c>
       <c r="D103">
         <v>3.26803173677304</v>
@@ -2496,7 +2497,7 @@
         <v>-0.03</v>
       </c>
       <c r="C104">
-        <v>0.133983294848767</v>
+        <v>87.007655425362202</v>
       </c>
       <c r="D104">
         <v>2.82817098511783</v>
@@ -2516,7 +2517,7 @@
         <v>-0.18</v>
       </c>
       <c r="C105">
-        <v>0.16844123061740399</v>
+        <v>87.150485146328194</v>
       </c>
       <c r="D105">
         <v>2.1845728046269599</v>
@@ -2536,7 +2537,7 @@
         <v>0.28000000000000003</v>
       </c>
       <c r="C106">
-        <v>0.24489486573411301</v>
+        <v>87.330054304190199</v>
       </c>
       <c r="D106">
         <v>3.7044060077008298</v>
@@ -2556,7 +2557,7 @@
         <v>0.21</v>
       </c>
       <c r="C107">
-        <v>0.32604381272801902</v>
+        <v>87.545950096286205</v>
       </c>
       <c r="D107">
         <v>3.4346305208982701</v>
@@ -2576,7 +2577,7 @@
         <v>0.59</v>
       </c>
       <c r="C108">
-        <v>5.5106020214960298E-2</v>
+        <v>87.786614048087401</v>
       </c>
       <c r="D108">
         <v>3.4753593527569899</v>
@@ -2596,7 +2597,7 @@
         <v>-7.0000000000000007E-2</v>
       </c>
       <c r="C109">
-        <v>-3.7187845693987302E-2</v>
+        <v>87.996317800257202</v>
       </c>
       <c r="D109">
         <v>2.98265388398264</v>
@@ -2616,7 +2617,7 @@
         <v>0.5</v>
       </c>
       <c r="C110">
-        <v>0.36824954321988701</v>
+        <v>88.245237805293399</v>
       </c>
       <c r="D110">
         <v>3.2836052762844199</v>
@@ -2636,7 +2637,7 @@
         <v>0.28999999999999998</v>
       </c>
       <c r="C111">
-        <v>0.341562743386915</v>
+        <v>88.314588652467606</v>
       </c>
       <c r="D111">
         <v>2.8574743632656401</v>
@@ -2656,7 +2657,7 @@
         <v>0.87</v>
       </c>
       <c r="C112">
-        <v>0.46758250493298598</v>
+        <v>88.513146732770096</v>
       </c>
       <c r="D112">
         <v>3.04048574612399</v>
@@ -2676,7 +2677,7 @@
         <v>0.61</v>
       </c>
       <c r="C113">
-        <v>8.9823424832237403E-2</v>
+        <v>88.570939105415405</v>
       </c>
       <c r="D113">
         <v>2.24101388446512</v>
@@ -2696,7 +2697,7 @@
         <v>0.84</v>
       </c>
       <c r="C114">
-        <v>5.6263629980605398E-2</v>
+        <v>88.726152906234006</v>
       </c>
       <c r="D114">
         <v>2.4627692895930999</v>
@@ -2716,7 +2717,7 @@
         <v>1.01</v>
       </c>
       <c r="C115">
-        <v>0.173343247513703</v>
+        <v>88.927600605168706</v>
       </c>
       <c r="D115">
         <v>4.0537008954527201</v>
@@ -2736,7 +2737,7 @@
         <v>0.53</v>
       </c>
       <c r="C116">
-        <v>0.22825012873863701</v>
+        <v>89.150926845176301</v>
       </c>
       <c r="D116">
         <v>3.9891287392789199</v>
@@ -2756,7 +2757,7 @@
         <v>-0.4</v>
       </c>
       <c r="C117">
-        <v>0.19949547547965699</v>
+        <v>89.327606384405996</v>
       </c>
       <c r="D117">
         <v>2.9401312849012702</v>
@@ -2776,7 +2777,7 @@
         <v>-0.14000000000000001</v>
       </c>
       <c r="C118">
-        <v>0.178310759622309</v>
+        <v>89.459703236166504</v>
       </c>
       <c r="D118">
         <v>3.1743897076137202</v>
@@ -2796,7 +2797,7 @@
         <v>-1.01</v>
       </c>
       <c r="C119">
-        <v>7.4240761405872505E-2</v>
+        <v>89.490663435797799</v>
       </c>
       <c r="D119">
         <v>2.2017102421699102</v>
@@ -2816,7 +2817,7 @@
         <v>-1.92</v>
       </c>
       <c r="C120">
-        <v>-0.153439957976817</v>
+        <v>89.556299059016396</v>
       </c>
       <c r="D120">
         <v>1.93625366578525</v>
@@ -2836,7 +2837,7 @@
         <v>-1.03</v>
       </c>
       <c r="C121">
-        <v>-0.27227837002168698</v>
+        <v>89.547217400457797</v>
       </c>
       <c r="D121">
         <v>0.36348415080054203</v>
@@ -2856,7 +2857,7 @@
         <v>0.44</v>
       </c>
       <c r="C122">
-        <v>0.28644146228598399</v>
+        <v>89.721007321055197</v>
       </c>
       <c r="D122">
         <v>2.4036406250263198</v>
@@ -2876,7 +2877,7 @@
         <v>0.5</v>
       </c>
       <c r="C123">
-        <v>0.44573849085681999</v>
+        <v>89.905117308196395</v>
       </c>
       <c r="D123">
         <v>2.1435760571947302</v>
@@ -2896,7 +2897,7 @@
         <v>0.24</v>
       </c>
       <c r="C124">
-        <v>0.43824792705056398</v>
+        <v>90.095419335263898</v>
       </c>
       <c r="D124">
         <v>1.9082898308551799</v>
@@ -2916,7 +2917,7 @@
         <v>0.25</v>
       </c>
       <c r="C125">
-        <v>0.23051697089721701</v>
+        <v>90.282418941037307</v>
       </c>
       <c r="D125">
         <v>1.8611701994373899</v>
@@ -2936,7 +2937,7 @@
         <v>0.28999999999999998</v>
       </c>
       <c r="C126">
-        <v>-6.8448456031046699E-3</v>
+        <v>90.364153868064193</v>
       </c>
       <c r="D126">
         <v>1.2937689372074099</v>
@@ -2956,7 +2957,7 @@
         <v>0.86</v>
       </c>
       <c r="C127">
-        <v>7.0734912927605795E-2</v>
+        <v>90.450016821708502</v>
       </c>
       <c r="D127">
         <v>0.75584590889346004</v>
@@ -2976,7 +2977,7 @@
         <v>-0.16</v>
       </c>
       <c r="C128">
-        <v>3.0554124122707398E-2</v>
+        <v>90.512350023633005</v>
       </c>
       <c r="D128">
         <v>0.12583251339235399</v>
@@ -2996,7 +2997,7 @@
         <v>0.22</v>
       </c>
       <c r="C129">
-        <v>0.112149532710279</v>
+        <v>90.608533043821097</v>
       </c>
       <c r="D129">
         <v>1.6255061079099</v>
@@ -3016,7 +3017,7 @@
         <v>0.06</v>
       </c>
       <c r="C130">
-        <v>0.24636150020949699</v>
+        <v>90.783561372403696</v>
       </c>
       <c r="D130">
         <v>0.914369783533586</v>
@@ -3036,7 +3037,7 @@
         <v>0.1</v>
       </c>
       <c r="C131">
-        <v>0.26983196827429401</v>
+        <v>91.023399718881393</v>
       </c>
       <c r="D131">
         <v>1.1903654188135</v>
@@ -3056,7 +3057,7 @@
         <v>7.0000000000000007E-2</v>
       </c>
       <c r="C132">
-        <v>-0.15720492364009001</v>
+        <v>91.091512158070401</v>
       </c>
       <c r="D132">
         <v>0.51601642131349201</v>
@@ -3076,7 +3077,7 @@
         <v>-0.18</v>
       </c>
       <c r="C133">
-        <v>-0.162897488020912</v>
+        <v>91.180264730347005</v>
       </c>
       <c r="D133">
         <v>0.46081040984140598</v>
@@ -3096,7 +3097,7 @@
         <v>0.34</v>
       </c>
       <c r="C134">
-        <v>2.7724122258833001E-2</v>
+        <v>91.077889670232594</v>
       </c>
       <c r="D134">
         <v>0.68011084594070703</v>
@@ -3116,7 +3117,7 @@
         <v>0.02</v>
       </c>
       <c r="C135">
-        <v>0.23445380442191699</v>
+        <v>91.118344331084302</v>
       </c>
       <c r="D135">
         <v>-0.10662785426794801</v>
@@ -3136,7 +3137,7 @@
         <v>0.41</v>
       </c>
       <c r="C136">
-        <v>0.20716040652395601</v>
+        <v>91.139810069495297</v>
       </c>
       <c r="D136">
         <v>-0.286064246298046</v>
@@ -3156,7 +3157,7 @@
         <v>0.17</v>
       </c>
       <c r="C137">
-        <v>4.8403367426812102E-2</v>
+        <v>91.155909373303601</v>
       </c>
       <c r="D137">
         <v>0.45261625417847201</v>
@@ -3176,7 +3177,7 @@
         <v>0.08</v>
       </c>
       <c r="C138">
-        <v>1.22080247415893E-2</v>
+        <v>91.213701745948896</v>
       </c>
       <c r="D138">
         <v>0.27574788971957997</v>
@@ -3196,7 +3197,7 @@
         <v>-0.1</v>
       </c>
       <c r="C139">
-        <v>3.25507588395616E-2</v>
+        <v>91.309471963475204</v>
       </c>
       <c r="D139">
         <v>1.26475267675238</v>
@@ -3216,7 +3217,7 @@
         <v>0.02</v>
       </c>
       <c r="C140">
-        <v>-3.1636273247027998E-3</v>
+        <v>91.379235613311195</v>
       </c>
       <c r="D140">
         <v>0.63230506844271805</v>
@@ -3236,7 +3237,7 @@
         <v>0.14000000000000001</v>
       </c>
       <c r="C141">
-        <v>0.13242459029730599</v>
+        <v>91.439504801927001</v>
       </c>
       <c r="D141">
         <v>0.43020593403721902</v>
@@ -3256,7 +3257,7 @@
         <v>0.06</v>
       </c>
       <c r="C142">
-        <v>0.160685350099986</v>
+        <v>91.522890939600799</v>
       </c>
       <c r="D142">
         <v>1.53627227687154</v>
@@ -3276,7 +3277,7 @@
         <v>0.12</v>
       </c>
       <c r="C143">
-        <v>7.7509947861027606E-2</v>
+        <v>91.572014456349194</v>
       </c>
       <c r="D143">
         <v>1.1260905710720199</v>
@@ -3296,7 +3297,7 @@
         <v>0.04</v>
       </c>
       <c r="C144">
-        <v>-9.0058042408725099E-4</v>
+        <v>91.703698505448003</v>
       </c>
       <c r="D144">
         <v>1.31829898066591</v>
@@ -3316,7 +3317,7 @@
         <v>0.17</v>
       </c>
       <c r="C145">
-        <v>-0.12698298337963601</v>
+        <v>91.783782221827806</v>
       </c>
       <c r="D145">
         <v>1.3933802807539999</v>
@@ -3336,7 +3337,7 @@
         <v>0.48</v>
       </c>
       <c r="C146">
-        <v>0.17223111431726301</v>
+        <v>91.973671446233496</v>
       </c>
       <c r="D146">
         <v>2.27322625990496</v>
@@ -3356,7 +3357,7 @@
         <v>0.49</v>
       </c>
       <c r="C147">
-        <v>0.375376389095185</v>
+        <v>92.142920537551603</v>
       </c>
       <c r="D147">
         <v>2.8169688979258898</v>
@@ -3376,7 +3377,7 @@
         <v>0.98</v>
       </c>
       <c r="C148">
-        <v>0.30446928626839198</v>
+        <v>92.242405979033805</v>
       </c>
       <c r="D148">
         <v>1.74418998266395</v>
@@ -3396,7 +3397,7 @@
         <v>0.64</v>
       </c>
       <c r="C149">
-        <v>0.191336224238907</v>
+        <v>92.355101105691901</v>
       </c>
       <c r="D149">
         <v>2.24921919600376</v>
@@ -3416,7 +3417,7 @@
         <v>0.47</v>
       </c>
       <c r="C150">
-        <v>0.185616505590811</v>
+        <v>92.540036698156598</v>
       </c>
       <c r="D150">
         <v>2.30581553962389</v>
@@ -3436,7 +3437,7 @@
         <v>-0.11</v>
       </c>
       <c r="C151">
-        <v>0.15899596497634999</v>
+        <v>92.755519687591004</v>
       </c>
       <c r="D151">
         <v>1.9267280763247201</v>
@@ -3456,7 +3457,7 @@
         <v>0.09</v>
       </c>
       <c r="C152">
-        <v>0.121392141081683</v>
+        <v>92.970589874363498</v>
       </c>
       <c r="D152">
         <v>2.5370313756664999</v>
@@ -3476,7 +3477,7 @@
         <v>0.28000000000000003</v>
       </c>
       <c r="C153">
-        <v>0.31532571814320998</v>
+        <v>93.236434788531497</v>
       </c>
       <c r="D153">
         <v>3.177970771699</v>
@@ -3496,7 +3497,7 @@
         <v>0.15</v>
       </c>
       <c r="C154">
-        <v>0.183730752543457</v>
+        <v>93.342112269939904</v>
       </c>
       <c r="D154">
         <v>2.4919770794244598</v>
@@ -3516,7 +3517,7 @@
         <v>-0.21</v>
       </c>
       <c r="C155">
-        <v>0.20062839996641099</v>
+        <v>93.502279702699497</v>
       </c>
       <c r="D155">
         <v>2.02226514469577</v>
@@ -3536,7 +3537,7 @@
         <v>-0.08</v>
       </c>
       <c r="C156">
-        <v>5.1159241961172802E-2</v>
+        <v>93.6645111487679</v>
       </c>
       <c r="D156">
         <v>1.84701379887521</v>
@@ -3556,7 +3557,7 @@
         <v>-0.25</v>
       </c>
       <c r="C157">
-        <v>-5.2455489973940402E-2</v>
+        <v>93.873389295614203</v>
       </c>
       <c r="D157">
         <v>2.37433305779156</v>
@@ -3576,7 +3577,7 @@
         <v>0.44</v>
       </c>
       <c r="C158">
-        <v>0.21919379024431601</v>
+        <v>94.068232151960899</v>
       </c>
       <c r="D158">
         <v>3.1980892845025402</v>
@@ -3596,7 +3597,7 @@
         <v>0.44</v>
       </c>
       <c r="C159">
-        <v>0.27636344433346</v>
+        <v>94.133042169855898</v>
       </c>
       <c r="D159">
         <v>1.6845519133678299</v>
@@ -3616,7 +3617,7 @@
         <v>0.76</v>
       </c>
       <c r="C160">
-        <v>0.38180501612795997</v>
+        <v>94.316326551673598</v>
       </c>
       <c r="D160">
         <v>2.4202963205617301</v>
@@ -3636,7 +3637,7 @@
         <v>0.3</v>
       </c>
       <c r="C161">
-        <v>0.24832229435810199</v>
+        <v>94.492593288241494</v>
       </c>
       <c r="D161">
         <v>2.2851338427891599</v>
@@ -3656,7 +3657,7 @@
         <v>-0.12</v>
       </c>
       <c r="C162">
-        <v>0.13039515401019</v>
+        <v>94.624277337340303</v>
       </c>
       <c r="D162">
         <v>1.7320720722101199</v>
@@ -3676,7 +3677,7 @@
         <v>-0.15</v>
       </c>
       <c r="C163">
-        <v>0.12064354840114599</v>
+        <v>94.788985599379103</v>
       </c>
       <c r="D163">
         <v>1.9220632776114399</v>
@@ -3696,7 +3697,7 @@
         <v>-0.16</v>
       </c>
       <c r="C164">
-        <v>6.0901604757317099E-3</v>
+        <v>94.932228123006894</v>
       </c>
       <c r="D164">
         <v>2.0837111943212201</v>
@@ -3716,7 +3717,7 @@
         <v>0.56000000000000005</v>
       </c>
       <c r="C165">
-        <v>0.131800446294594</v>
+        <v>95.040795223047596</v>
       </c>
       <c r="D165">
         <v>2.4238660191344499</v>
@@ -3736,7 +3737,7 @@
         <v>0.45</v>
       </c>
       <c r="C166">
-        <v>0.25369684964116102</v>
+        <v>95.216649156953807</v>
       </c>
       <c r="D166">
         <v>2.2866037427289299</v>
@@ -3756,7 +3757,7 @@
         <v>-0.04</v>
       </c>
       <c r="C167">
-        <v>0.21492330357918299</v>
+        <v>95.3673221284931</v>
       </c>
       <c r="D167">
         <v>1.8750476631537301</v>
@@ -3776,7 +3777,7 @@
         <v>-0.47</v>
       </c>
       <c r="C168">
-        <v>-5.6209896400966101E-3</v>
+        <v>95.493639742989103</v>
       </c>
       <c r="D168">
         <v>2.0721553787935498</v>
@@ -3796,7 +3797,7 @@
         <v>-0.27</v>
       </c>
       <c r="C169">
-        <v>-9.9453868539285797E-2</v>
+        <v>95.656696794380906</v>
       </c>
       <c r="D169">
         <v>1.7906501656690199</v>
@@ -3816,7 +3817,7 @@
         <v>0.3</v>
       </c>
       <c r="C170">
-        <v>0.25061354871383101</v>
+        <v>95.864749335903696</v>
       </c>
       <c r="D170">
         <v>2.7418075036870402</v>
@@ -3836,7 +3837,7 @@
         <v>0.82</v>
       </c>
       <c r="C171">
-        <v>0.35404037787331699</v>
+        <v>96.005102240899205</v>
       </c>
       <c r="D171">
         <v>2.45154222786008</v>
@@ -3856,7 +3857,7 @@
         <v>0.26</v>
       </c>
       <c r="C172">
-        <v>0.26674468231569498</v>
+        <v>96.097982839793403</v>
       </c>
       <c r="D172">
         <v>1.2153579117970299</v>
@@ -3876,7 +3877,7 @@
         <v>-0.1</v>
       </c>
       <c r="C173">
-        <v>7.89523368175441E-2</v>
+        <v>96.113669340939893</v>
       </c>
       <c r="D173">
         <v>2.0888841859939999</v>
@@ -3896,7 +3897,7 @@
         <v>0.18</v>
       </c>
       <c r="C174">
-        <v>9.6897562983423599E-2</v>
+        <v>96.181368977467201</v>
       </c>
       <c r="D174">
         <v>1.9563823322528999</v>
@@ -3916,7 +3917,7 @@
         <v>0.24</v>
       </c>
       <c r="C175">
-        <v>7.6243671346929998E-2</v>
+        <v>96.327501119727202</v>
       </c>
       <c r="D175">
         <v>2.1372504396246899</v>
@@ -3936,7 +3937,7 @@
         <v>0.04</v>
       </c>
       <c r="C176">
-        <v>6.5057353192953998E-2</v>
+        <v>96.546286530455603</v>
       </c>
       <c r="D176">
         <v>2.0032000474006901</v>
@@ -3956,7 +3957,7 @@
         <v>0.12</v>
       </c>
       <c r="C177">
-        <v>0.19932247467835401</v>
+        <v>96.734524544214295</v>
       </c>
       <c r="D177">
         <v>2.1480298989161999</v>
@@ -3976,7 +3977,7 @@
         <v>0.12</v>
       </c>
       <c r="C178">
-        <v>0.223684996883766</v>
+        <v>96.884784713091804</v>
       </c>
       <c r="D178">
         <v>2.2321601731445599</v>
@@ -3996,7 +3997,7 @@
         <v>-0.26</v>
       </c>
       <c r="C179">
-        <v>0.161852271468859</v>
+        <v>96.976014101338905</v>
       </c>
       <c r="D179">
         <v>1.1637292908921699</v>
@@ -4016,7 +4017,7 @@
         <v>-0.2</v>
       </c>
       <c r="C180">
-        <v>3.4444340497179399E-2</v>
+        <v>97.156821667186094</v>
       </c>
       <c r="D180">
         <v>2.6055064073774199</v>
@@ -4036,7 +4037,7 @@
         <v>-0.01</v>
       </c>
       <c r="C181">
-        <v>-0.10329744136913099</v>
+        <v>97.321942731886793</v>
       </c>
       <c r="D181">
         <v>2.8446440822717198</v>
@@ -4056,7 +4057,7 @@
         <v>0.37</v>
       </c>
       <c r="C182">
-        <v>0.15617021276596399</v>
+        <v>97.405328869560606</v>
       </c>
       <c r="D182">
         <v>2.4063265035218699</v>
@@ -4076,7 +4077,7 @@
         <v>0.37</v>
       </c>
       <c r="C183">
-        <v>0.300806825085917</v>
+        <v>97.497796665792904</v>
       </c>
       <c r="D183">
         <v>2.3508313464702399</v>
@@ -4096,7 +4097,7 @@
         <v>0.64</v>
       </c>
       <c r="C184">
-        <v>0.35497193688447598</v>
+        <v>97.679429836963607</v>
       </c>
       <c r="D184">
         <v>2.8589766754357</v>
@@ -4116,7 +4117,7 @@
         <v>0.33</v>
       </c>
       <c r="C185">
-        <v>0.251569141414755</v>
+        <v>97.863952626766505</v>
       </c>
       <c r="D185">
         <v>2.2149322287967599</v>
@@ -4136,7 +4137,7 @@
         <v>0.35</v>
       </c>
       <c r="C186">
-        <v>0.218939071782558</v>
+        <v>98.052603443186996</v>
       </c>
       <c r="D186">
         <v>2.5456266070807101</v>
@@ -4156,7 +4157,7 @@
         <v>0.19</v>
       </c>
       <c r="C187">
-        <v>5.3774960193923298E-2</v>
+        <v>98.179746663006497</v>
       </c>
       <c r="D187">
         <v>1.31136444111866</v>
@@ -4176,7 +4177,7 @@
         <v>-0.04</v>
       </c>
       <c r="C188">
-        <v>-7.9779305248114992E-3</v>
+        <v>98.327530015913496</v>
       </c>
       <c r="D188">
         <v>2.40490383837574</v>
@@ -4196,7 +4197,7 @@
         <v>-0.17</v>
       </c>
       <c r="C189">
-        <v>6.6348083884141595E-2</v>
+        <v>98.414218574881403</v>
       </c>
       <c r="D189">
         <v>1.7517369153509701</v>
@@ -4216,7 +4217,7 @@
         <v>0.08</v>
       </c>
       <c r="C190">
-        <v>0.22870715412762199</v>
+        <v>98.571496389008701</v>
       </c>
       <c r="D190">
         <v>1.9354109845871399</v>
@@ -4236,7 +4237,7 @@
         <v>-0.25</v>
       </c>
       <c r="C191">
-        <v>0.239489869829728</v>
+        <v>98.738681467018097</v>
       </c>
       <c r="D191">
         <v>2.4289565511268001</v>
@@ -4256,7 +4257,7 @@
         <v>-0.54</v>
       </c>
       <c r="C192">
-        <v>-6.8918563319460793E-2</v>
+        <v>98.848899777705796</v>
       </c>
       <c r="D192">
         <v>2.2563105410023301</v>
@@ -4276,7 +4277,7 @@
         <v>-0.56999999999999995</v>
       </c>
       <c r="C193">
-        <v>-0.197702802113285</v>
+        <v>98.900912913086501</v>
       </c>
       <c r="D193">
         <v>2.3833942455642001</v>
@@ -4296,7 +4297,7 @@
         <v>-0.47</v>
       </c>
       <c r="C194">
-        <v>0.19809444037273299</v>
+        <v>98.994619117304097</v>
       </c>
       <c r="D194">
         <v>1.9475295988382599</v>
@@ -4316,7 +4317,7 @@
         <v>0.43</v>
       </c>
       <c r="C195">
-        <v>0.349010232060461</v>
+        <v>99.143640878196393</v>
       </c>
       <c r="D195">
         <v>1.95449451571832</v>
@@ -4336,7 +4337,7 @@
         <v>0.6</v>
       </c>
       <c r="C196">
-        <v>0.40985825735267301</v>
+        <v>99.384304829997603</v>
       </c>
       <c r="D196">
         <v>2.4333359263674299</v>
@@ -4356,7 +4357,7 @@
         <v>0.2</v>
       </c>
       <c r="C197">
-        <v>0.30489448991357299</v>
+        <v>99.628271203092694</v>
       </c>
       <c r="D197">
         <v>2.96265053867684</v>
@@ -4376,7 +4377,7 @@
         <v>0.51</v>
       </c>
       <c r="C198">
-        <v>0.13109899835404101</v>
+        <v>99.769449713411802</v>
       </c>
       <c r="D198">
         <v>2.5012910991094999</v>
@@ -4396,7 +4397,7 @@
         <v>0.35</v>
       </c>
       <c r="C199">
-        <v>9.70597103077315E-2</v>
+        <v>99.924663514230403</v>
       </c>
       <c r="D199">
         <v>2.9723995643109098</v>
@@ -4416,7 +4417,7 @@
         <v>0.01</v>
       </c>
       <c r="C200">
-        <v>3.38348036343675E-2</v>
+        <v>100.13147764776799</v>
       </c>
       <c r="D200">
         <v>1.92202530060316</v>
@@ -4436,7 +4437,7 @@
         <v>-0.14000000000000001</v>
       </c>
       <c r="C201">
-        <v>8.8683198864853693E-2</v>
+        <v>100.23550391852901</v>
       </c>
       <c r="D201">
         <v>1.6357906321156499</v>
@@ -4456,7 +4457,7 @@
         <v>-0.16</v>
       </c>
       <c r="C202">
-        <v>0.29177707901472599</v>
+        <v>100.441492446743</v>
       </c>
       <c r="D202">
         <v>2.99841569275871</v>
@@ -4476,7 +4477,7 @@
         <v>-0.04</v>
       </c>
       <c r="C203">
-        <v>0.257233141161818</v>
+        <v>100.62807924985501</v>
       </c>
       <c r="D203">
         <v>2.28316449144805</v>
@@ -4496,7 +4497,7 @@
         <v>-0.21</v>
       </c>
       <c r="C204">
-        <v>3.68875135766389E-2</v>
+        <v>100.823334908864</v>
       </c>
       <c r="D204">
         <v>2.2654806001265002</v>
@@ -4516,7 +4517,7 @@
         <v>-0.34</v>
       </c>
       <c r="C205">
-        <v>-0.12127419850455801</v>
+        <v>100.94965252335901</v>
       </c>
       <c r="D205">
         <v>1.83471969623819</v>
@@ -4536,7 +4537,7 @@
         <v>0.17</v>
       </c>
       <c r="C206">
-        <v>0.30724549694601</v>
+        <v>101.118076009354</v>
       </c>
       <c r="D206">
         <v>2.7084165913200402</v>
@@ -4556,7 +4557,7 @@
         <v>0.08</v>
       </c>
       <c r="C207">
-        <v>0.47111169273049502</v>
+        <v>101.347181486626</v>
       </c>
       <c r="D207">
         <v>2.5377144012724799</v>
@@ -4576,7 +4577,7 @@
         <v>0.43</v>
       </c>
       <c r="C208">
-        <v>0.27596873982414</v>
+        <v>101.513540959312</v>
       </c>
       <c r="D208">
         <v>2.2220045586459198</v>
@@ -4596,7 +4597,7 @@
         <v>0.47</v>
       </c>
       <c r="C209">
-        <v>0.25734906112244099</v>
+        <v>101.77690905751</v>
       </c>
       <c r="D209">
         <v>3.8254778833095</v>
@@ -4616,7 +4617,7 @@
         <v>0.4</v>
       </c>
       <c r="C210">
-        <v>0.22348901988730099</v>
+        <v>102.01881141729601</v>
       </c>
       <c r="D210">
         <v>3.2805191880404001</v>
@@ -4636,7 +4637,7 @@
         <v>0.33</v>
       </c>
       <c r="C211">
-        <v>0.100992146850645</v>
+        <v>102.185170889982</v>
       </c>
       <c r="D211">
         <v>2.1033904605521201</v>
@@ -4656,7 +4657,7 @@
         <v>-0.16</v>
       </c>
       <c r="C212">
-        <v>-2.0178051123111499E-2</v>
+        <v>102.304470859228</v>
       </c>
       <c r="D212">
         <v>2.4901647109793599</v>
@@ -4676,7 +4677,7 @@
         <v>0.09</v>
       </c>
       <c r="C213">
-        <v>0.215545078791017</v>
+        <v>102.549675640309</v>
       </c>
       <c r="D213">
         <v>2.7425708907920798</v>
@@ -4696,7 +4697,7 @@
         <v>0.24</v>
       </c>
       <c r="C214">
-        <v>0.182456762177865</v>
+        <v>102.722639955582</v>
       </c>
       <c r="D214">
         <v>2.4983293349312201</v>
@@ -4716,7 +4717,7 @@
         <v>0.12</v>
       </c>
       <c r="C215">
-        <v>0.195793849580471</v>
+        <v>102.846480754108</v>
       </c>
       <c r="D215">
         <v>2.0180255617507501</v>
@@ -4736,7 +4737,7 @@
         <v>-0.16</v>
       </c>
       <c r="C216">
-        <v>3.6112961343130801E-3</v>
+        <v>102.986420856442</v>
       </c>
       <c r="D216">
         <v>2.45883151623452</v>
@@ -4756,7 +4757,7 @@
         <v>0.03</v>
       </c>
       <c r="C217">
-        <v>-3.7315379152339997E-2</v>
+        <v>103.167641224951</v>
       </c>
       <c r="D217">
         <v>2.0383851077488102</v>
@@ -4776,7 +4777,7 @@
         <v>0.57999999999999996</v>
       </c>
       <c r="C218">
-        <v>0.380919505165905</v>
+        <v>103.393444280929</v>
       </c>
       <c r="D218">
         <v>3.4363057748294299</v>
@@ -4796,7 +4797,7 @@
         <v>0.31</v>
       </c>
       <c r="C219">
-        <v>0.42385927871946499</v>
+        <v>103.612642494319</v>
       </c>
       <c r="D219">
         <v>3.2923463387532199</v>
@@ -4816,7 +4817,7 @@
         <v>0.08</v>
       </c>
       <c r="C220">
-        <v>5.8532389913325399E-2</v>
+        <v>103.590351150584</v>
       </c>
       <c r="D220">
         <v>1.9143836751172301</v>
@@ -4836,7 +4837,7 @@
         <v>0.3</v>
       </c>
       <c r="C221">
-        <v>0.14007720163953</v>
+        <v>103.70717430386</v>
       </c>
       <c r="D221">
         <v>1.5536583625790099</v>
@@ -4856,7 +4857,7 @@
         <v>0.09</v>
       </c>
       <c r="C222">
-        <v>7.6696258971081302E-2</v>
+        <v>103.790973244195</v>
       </c>
       <c r="D222">
         <v>2.1132188709843498</v>
@@ -4876,7 +4877,7 @@
         <v>0.09</v>
       </c>
       <c r="C223">
-        <v>7.1078285385272597E-2</v>
+        <v>103.921418885309</v>
       </c>
       <c r="D223">
         <v>1.89683378620466</v>
@@ -4896,7 +4897,7 @@
         <v>-7.0000000000000007E-2</v>
       </c>
       <c r="C224">
-        <v>-3.0950661471195101E-2</v>
+        <v>104.020078721468</v>
       </c>
       <c r="D224">
         <v>2.1220936834140698</v>
@@ -4916,7 +4917,7 @@
         <v>0.3</v>
       </c>
       <c r="C225">
-        <v>0.20798933062364</v>
+        <v>104.247120185431</v>
       </c>
       <c r="D225">
         <v>2.2747579876520398</v>
@@ -4936,7 +4937,7 @@
         <v>0.53</v>
       </c>
       <c r="C226">
-        <v>0.190525231719887</v>
+        <v>104.36146652273599</v>
       </c>
       <c r="D226">
         <v>2.8702567714482998</v>
@@ -4956,7 +4957,7 @@
         <v>-0.06</v>
       </c>
       <c r="C227">
-        <v>0.27555833178488298</v>
+        <v>104.656207623227</v>
       </c>
       <c r="D227">
         <v>2.4249630240346498</v>
@@ -4976,7 +4977,7 @@
         <v>0</v>
       </c>
       <c r="C228">
-        <v>-5.75623526443165E-2</v>
+        <v>104.775920395135</v>
       </c>
       <c r="D228">
         <v>2.4203929586135802</v>
@@ -4996,7 +4997,7 @@
         <v>-0.06</v>
       </c>
       <c r="C229">
-        <v>2.60363246177257E-2</v>
+        <v>104.99388020054</v>
       </c>
       <c r="D229">
         <v>2.9557471890823401</v>
@@ -5016,7 +5017,7 @@
         <v>0.54</v>
       </c>
       <c r="C230">
-        <v>0.42593804967700999</v>
+        <v>105.348890489646</v>
       </c>
       <c r="D230">
         <v>4.17000041826154</v>
@@ -5036,7 +5037,7 @@
         <v>0.45</v>
       </c>
       <c r="C231">
-        <v>0.44965794578971702</v>
+        <v>105.558181439154</v>
       </c>
       <c r="D231">
         <v>2.0132793455486699</v>
@@ -5056,7 +5057,7 @@
         <v>0.23</v>
       </c>
       <c r="C232">
-        <v>0.32332094001555101</v>
+        <v>105.78935092973499</v>
       </c>
       <c r="D232">
         <v>1.96190007372538</v>
@@ -5076,7 +5077,7 @@
         <v>0.4</v>
       </c>
       <c r="C233">
-        <v>0.16172401699074701</v>
+        <v>105.937547085304</v>
       </c>
       <c r="D233">
         <v>2.9320091480948798</v>
@@ -5096,7 +5097,7 @@
         <v>0.42</v>
       </c>
       <c r="C234">
-        <v>0.1727458418442</v>
+        <v>106.150140456106</v>
       </c>
       <c r="D234">
         <v>2.98183255084012</v>
@@ -5116,7 +5117,7 @@
         <v>0.16</v>
       </c>
       <c r="C235">
-        <v>8.8554350232465495E-2</v>
+        <v>106.25499233219099</v>
       </c>
       <c r="D235">
         <v>2.6321178885371199</v>
@@ -5136,7 +5137,7 @@
         <v>0.01</v>
       </c>
       <c r="C236">
-        <v>6.59689480281061E-2</v>
+        <v>106.378833130716</v>
       </c>
       <c r="D236">
         <v>2.1114939144998499</v>
@@ -5156,7 +5157,7 @@
         <v>0.06</v>
       </c>
       <c r="C237">
-        <v>5.6230537447583599E-2</v>
+        <v>106.458091241772</v>
       </c>
       <c r="D237">
         <v>2.2967112867850998</v>
@@ -5176,7 +5177,7 @@
         <v>0.12</v>
       </c>
       <c r="C238">
-        <v>0.16162038974929999</v>
+        <v>106.654998111428</v>
       </c>
       <c r="D238">
         <v>2.33372335554622</v>
@@ -5196,7 +5197,7 @@
         <v>0.18</v>
       </c>
       <c r="C239">
-        <v>0.24532850415395499</v>
+        <v>106.88162677272901</v>
       </c>
       <c r="D239">
         <v>2.6062626874792301</v>
@@ -5216,7 +5217,7 @@
         <v>-0.33</v>
       </c>
       <c r="C240">
-        <v>1.6212272690435101E-2</v>
+        <v>107.097109762164</v>
       </c>
       <c r="D240">
         <v>3.72376360170077</v>
@@ -5236,7 +5237,7 @@
         <v>-0.32</v>
       </c>
       <c r="C241">
-        <v>-8.4907662916533493E-3</v>
+        <v>107.35469862309699</v>
       </c>
       <c r="D241">
         <v>2.91177701505443</v>
@@ -5256,7 +5257,7 @@
         <v>0.19</v>
       </c>
       <c r="C242">
-        <v>0.40102978582152798</v>
+        <v>107.61187468136799</v>
       </c>
       <c r="D242">
         <v>3.23099390584713</v>
@@ -5276,7 +5277,7 @@
         <v>0.42</v>
       </c>
       <c r="C243">
-        <v>0.381359515919442</v>
+        <v>107.76915249549501</v>
       </c>
       <c r="D243">
         <v>3.0245121242261601</v>
@@ -5296,7 +5297,7 @@
         <v>0.56000000000000005</v>
       </c>
       <c r="C244">
-        <v>0.27650757906509399</v>
+        <v>107.963169746519</v>
       </c>
       <c r="D244">
         <v>3.2071444963092199</v>
@@ -5316,7 +5317,7 @@
         <v>0.53</v>
       </c>
       <c r="C245">
-        <v>0.18943155257489899</v>
+        <v>108.14439011502699</v>
       </c>
       <c r="D245">
         <v>2.2774968873232502</v>
@@ -5336,7 +5337,7 @@
         <v>0.21</v>
       </c>
       <c r="C246">
-        <v>9.8348657426445302E-2</v>
+        <v>108.27978938808199</v>
       </c>
       <c r="D246">
         <v>2.5585351456762702</v>
@@ -5356,7 +5357,7 @@
         <v>0.02</v>
       </c>
       <c r="C247">
-        <v>0.22354240450895299</v>
+        <v>108.50889486535399</v>
       </c>
       <c r="D247">
         <v>3.8073452144987501</v>
@@ -5376,7 +5377,7 @@
         <v>0.17</v>
       </c>
       <c r="C248">
-        <v>0.147809269047048</v>
+        <v>108.696307273789</v>
       </c>
       <c r="D248">
         <v>2.4690479946519699</v>
@@ -5396,7 +5397,7 @@
         <v>-0.01</v>
       </c>
       <c r="C249">
-        <v>0.22878519991198501</v>
+        <v>108.969582635869</v>
       </c>
       <c r="D249">
         <v>2.4628290795772898</v>
@@ -5416,7 +5417,7 @@
         <v>0.08</v>
       </c>
       <c r="C250">
-        <v>0.133626579954502</v>
+        <v>109.155343833657</v>
       </c>
       <c r="D250">
         <v>3.1506552025938999</v>
@@ -5436,7 +5437,7 @@
         <v>0.23</v>
       </c>
       <c r="C251">
-        <v>0.20300768934152999</v>
+        <v>109.367937204459</v>
       </c>
       <c r="D251">
         <v>2.5257194144135999</v>
@@ -5456,7 +5457,7 @@
         <v>-0.05</v>
       </c>
       <c r="C252">
-        <v>1.8486450186551599E-2</v>
+        <v>109.592501852452</v>
       </c>
       <c r="D252">
         <v>3.4502701963413398</v>
@@ -5476,7 +5477,7 @@
         <v>-0.09</v>
       </c>
       <c r="C253">
-        <v>-6.5256423797084601E-2</v>
+        <v>109.774135023623</v>
       </c>
       <c r="D253">
         <v>2.6123304640999399</v>
@@ -5496,7 +5497,7 @@
         <v>0.39</v>
       </c>
       <c r="C254">
-        <v>0.40349519693512198</v>
+        <v>110.063922492172</v>
       </c>
       <c r="D254">
         <v>3.2069756335673301</v>
@@ -5516,7 +5517,7 @@
         <v>0.27</v>
       </c>
       <c r="C255">
-        <v>0.47518082434847603</v>
+        <v>110.335133840943</v>
       </c>
       <c r="D255">
         <v>2.7086305355471301</v>
@@ -5536,7 +5537,7 @@
         <v>-0.22</v>
       </c>
       <c r="C256">
-        <v>1.6462876214148599E-2</v>
+        <v>110.255462927225</v>
       </c>
       <c r="D256">
         <v>2.9665443806796699</v>
@@ -5556,7 +5557,7 @@
         <v>-0.67</v>
       </c>
       <c r="C257">
-        <v>-0.457517806907278</v>
+        <v>109.710976216375</v>
       </c>
       <c r="D257">
         <v>1.9683735023159501</v>
@@ -5576,7 +5577,7 @@
         <v>0</v>
       </c>
       <c r="C258">
-        <v>-0.108986091119899</v>
+        <v>109.62965409201</v>
       </c>
       <c r="D258">
         <v>2.8950442655885298</v>
@@ -5596,7 +5597,7 @@
         <v>0.55000000000000004</v>
       </c>
       <c r="C259">
-        <v>0.18924074206449801</v>
+        <v>109.785693498152</v>
       </c>
       <c r="D259">
         <v>1.68037017264615</v>
@@ -5616,7 +5617,7 @@
         <v>0.51</v>
       </c>
       <c r="C260">
-        <v>0.52609443413866697</v>
+        <v>110.363617224604</v>
       </c>
       <c r="D260">
         <v>3.6108294731035202</v>
@@ -5636,7 +5637,7 @@
         <v>0.32</v>
       </c>
       <c r="C261">
-        <v>0.39334635771731902</v>
+        <v>110.82471779778</v>
       </c>
       <c r="D261">
         <v>2.2357232767131499</v>
@@ -5656,7 +5657,7 @@
         <v>0.14000000000000001</v>
       </c>
       <c r="C262">
-        <v>0.11088124544196599</v>
+        <v>111.01832224614201</v>
       </c>
       <c r="D262">
         <v>1.13393304399887</v>
@@ -5676,7 +5677,7 @@
         <v>0.04</v>
       </c>
       <c r="C263">
-        <v>0.10183829268474399</v>
+        <v>111.141337439344</v>
       </c>
       <c r="D263">
         <v>1.83845624148977</v>
@@ -5696,7 +5697,7 @@
         <v>-0.06</v>
       </c>
       <c r="C264">
-        <v>5.3837699756436097E-2</v>
+        <v>111.415851209409</v>
       </c>
       <c r="D264">
         <v>1.21891052470624</v>
@@ -5716,7 +5717,7 @@
         <v>0.09</v>
       </c>
       <c r="C265">
-        <v>-9.16603889814471E-2</v>
+        <v>111.56693698361001</v>
       </c>
       <c r="D265">
         <v>1.6244821427238201</v>
@@ -5736,7 +5737,7 @@
         <v>0.43</v>
       </c>
       <c r="C266">
-        <v>0.19648919495144199</v>
+        <v>111.614822092373</v>
       </c>
       <c r="D266">
         <v>1.52430226027722</v>
@@ -5756,7 +5757,7 @@
         <v>0.55000000000000004</v>
       </c>
       <c r="C267">
-        <v>0.348835054030526</v>
+        <v>111.756826208015</v>
       </c>
       <c r="D267">
         <v>2.8103907135000399</v>
@@ -5776,7 +5777,7 @@
         <v>0.71</v>
       </c>
       <c r="C268">
-        <v>0.37569820019505301</v>
+        <v>112.086655534755</v>
       </c>
       <c r="D268">
         <v>2.3566512577708498</v>
@@ -5796,7 +5797,7 @@
         <v>0.82</v>
       </c>
       <c r="C269">
-        <v>0.82991980508844598</v>
+        <v>112.94900029515399</v>
       </c>
       <c r="D269">
         <v>2.7458149440762001</v>
@@ -5816,7 +5817,7 @@
         <v>0.8</v>
       </c>
       <c r="C270">
-        <v>0.70263680429830599</v>
+        <v>113.790704922465</v>
       </c>
       <c r="D270">
         <v>3.33847353905972</v>
@@ -5836,7 +5837,7 @@
         <v>0.93</v>
       </c>
       <c r="C271">
-        <v>0.84271801024312298</v>
+        <v>114.62539190452701</v>
       </c>
       <c r="D271">
         <v>3.1694932706457499</v>
@@ -5856,7 +5857,7 @@
         <v>0.48</v>
       </c>
       <c r="C272">
-        <v>0.33355138776066301</v>
+        <v>114.974622956369</v>
       </c>
       <c r="D272">
         <v>3.5810454687451601</v>
@@ -5876,7 +5877,7 @@
         <v>0.21</v>
       </c>
       <c r="C273">
-        <v>0.129323006598693</v>
+        <v>115.195472380406</v>
       </c>
       <c r="D273">
         <v>4.0220376707694099</v>
@@ -5896,7 +5897,7 @@
         <v>0.27</v>
       </c>
       <c r="C274">
-        <v>0.134880342889446</v>
+        <v>115.48360863830899</v>
       </c>
       <c r="D274">
         <v>5.0542750166043602</v>
@@ -5916,7 +5917,7 @@
         <v>0.83</v>
       </c>
       <c r="C275">
-        <v>0.61918509096625896</v>
+        <v>116.240275917299</v>
       </c>
       <c r="D275">
         <v>7.6628525874679596</v>
@@ -5936,7 +5937,7 @@
         <v>0.49</v>
       </c>
       <c r="C276">
-        <v>0.403739831047145</v>
+        <v>116.963506180688</v>
       </c>
       <c r="D276">
         <v>6.24507044851239</v>
@@ -5956,7 +5957,7 @@
         <v>0.31</v>
       </c>
       <c r="C277">
-        <v>0.40812862063842698</v>
+        <v>117.728429512914</v>
       </c>
       <c r="D277">
         <v>5.6117970586782304</v>
@@ -5976,7 +5977,7 @@
         <v>0.84</v>
       </c>
       <c r="C278">
-        <v>0.73544951181367402</v>
+        <v>118.38850096905399</v>
       </c>
       <c r="D278">
         <v>6.9928263111253202</v>
@@ -5996,7 +5997,7 @@
         <v>0.91</v>
       </c>
       <c r="C279">
-        <v>0.72133875998267305</v>
+        <v>118.947848575728</v>
       </c>
       <c r="D279">
         <v>6.5195545827471602</v>
@@ -6016,7 +6017,7 @@
         <v>1.34</v>
       </c>
       <c r="C280">
-        <v>0.43255027615868602</v>
+        <v>119.318958168642</v>
       </c>
       <c r="D280">
         <v>6.3502494107233503</v>
@@ -6036,7 +6037,7 @@
         <v>0.56000000000000005</v>
       </c>
       <c r="C281">
-        <v>0.53265584763485796</v>
+        <v>119.88202099927101</v>
       </c>
       <c r="D281">
         <v>6.0303202233042503</v>
@@ -6056,7 +6057,7 @@
         <v>1.1000000000000001</v>
       </c>
       <c r="C282">
-        <v>0.57074878114190397</v>
+        <v>120.641990699556</v>
       </c>
       <c r="D282">
         <v>7.5039441135080303</v>
@@ -6076,7 +6077,7 @@
         <v>1.37</v>
       </c>
       <c r="C283">
-        <v>0.74323261745058899</v>
+        <v>121.371000200209</v>
       </c>
       <c r="D283">
         <v>7.9249191844640698</v>
@@ -6096,7 +6097,7 @@
         <v>-0.01</v>
       </c>
       <c r="C284">
-        <v>0.32781322112122302</v>
+        <v>121.74582501707999</v>
       </c>
       <c r="D284">
         <v>6.4236110188124496</v>
@@ -6116,7 +6117,7 @@
         <v>-0.04</v>
       </c>
       <c r="C285">
-        <v>0.51818729155813403</v>
+        <v>122.45336877932201</v>
       </c>
       <c r="D285">
         <v>8.4639174660262402</v>
@@ -6136,7 +6137,7 @@
         <v>0.22</v>
       </c>
       <c r="C286">
-        <v>0.42533431142279299</v>
+        <v>123.15513330429999</v>
       </c>
       <c r="D286">
         <v>8.3829643022701905</v>
@@ -6156,7 +6157,7 @@
         <v>0.41</v>
       </c>
       <c r="C287">
-        <v>0.292519149449462</v>
+        <v>123.565459150081</v>
       </c>
       <c r="D287">
         <v>6.5077480442296398</v>
@@ -6176,7 +6177,7 @@
         <v>-0.1</v>
       </c>
       <c r="C288">
-        <v>9.5217413093240694E-2</v>
+        <v>123.948540020186</v>
       </c>
       <c r="D288">
         <v>5.7657702180623698</v>
@@ -6196,7 +6197,7 @@
         <v>-0.31</v>
       </c>
       <c r="C289">
-        <v>0.17122830440585901</v>
+        <v>124.443490411626</v>
       </c>
       <c r="D289">
         <v>7.0491610305983796</v>
@@ -6216,7 +6217,7 @@
         <v>0.8</v>
       </c>
       <c r="C290">
-        <v>0.61610126852218094</v>
+        <v>124.956191317522</v>
       </c>
       <c r="D290">
         <v>8.1424953553777097</v>
@@ -6236,7 +6237,7 @@
         <v>0.56000000000000005</v>
       </c>
       <c r="C291">
-        <v>0.67856220319116101</v>
+        <v>125.520905358798</v>
       </c>
       <c r="D291">
         <v>7.8804958949669999</v>
@@ -6256,7 +6257,7 @@
         <v>0.33</v>
       </c>
       <c r="C292">
-        <v>0.48189045791105101</v>
+        <v>126.00388447304699</v>
       </c>
       <c r="D292">
         <v>4.9070545279561202</v>
@@ -6276,7 +6277,7 @@
         <v>0.51</v>
       </c>
       <c r="C293">
-        <v>0.46583037619976603</v>
+        <v>126.519474997575</v>
       </c>
       <c r="D293">
         <v>4.9115950802641102</v>
@@ -6296,7 +6297,7 @@
         <v>0.25</v>
       </c>
       <c r="C294">
-        <v>0.39003059638513998</v>
+        <v>127.070566551013</v>
       </c>
       <c r="D294">
         <v>4.6556863428989201</v>

</xml_diff>